<commit_message>
14:17 Uppdatering av koordinater + lite grafik
</commit_message>
<xml_diff>
--- a/Design/Tutorial_koordinater.xlsx
+++ b/Design/Tutorial_koordinater.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Tutorial 02</t>
   </si>
@@ -25,9 +25,6 @@
   </si>
   <si>
     <t>Hus02</t>
-  </si>
-  <si>
-    <t>Exit</t>
   </si>
   <si>
     <t>Hinder</t>
@@ -109,7 +106,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -119,15 +116,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -167,6 +155,82 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -174,55 +238,14 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -231,9 +254,7 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -244,23 +265,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,225 +596,226 @@
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="9" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1088</v>
+      </c>
+      <c r="C4" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1180</v>
+      </c>
+      <c r="C5" s="3">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2">
+        <v>544</v>
+      </c>
+      <c r="C6" s="3">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2">
+        <v>400</v>
+      </c>
+      <c r="C7" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2">
+        <v>720</v>
+      </c>
+      <c r="C8" s="3">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2">
+        <v>64</v>
+      </c>
+      <c r="C9" s="3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4">
+        <v>896</v>
+      </c>
+      <c r="C10" s="5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="17" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="B12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B13" s="13">
         <v>0</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C13" s="1">
         <v>480</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1088</v>
-      </c>
-      <c r="C3" s="4">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="14">
+        <v>320</v>
+      </c>
+      <c r="C14" s="3">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="14">
+        <v>576</v>
+      </c>
+      <c r="C15" s="3">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="14">
+        <v>960</v>
+      </c>
+      <c r="C16" s="3">
         <v>480</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3">
-        <v>1216</v>
-      </c>
-      <c r="C4" s="4">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3">
-        <v>544</v>
-      </c>
-      <c r="C5" s="4">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3">
-        <v>400</v>
-      </c>
-      <c r="C6" s="4">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3">
-        <v>720</v>
-      </c>
-      <c r="C7" s="4">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3">
-        <v>64</v>
-      </c>
-      <c r="C8" s="4">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="5">
-        <v>896</v>
-      </c>
-      <c r="C9" s="6">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:3" ht="32.25" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="1">
-        <v>0</v>
-      </c>
-      <c r="C12" s="2">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="15">
-        <v>320</v>
-      </c>
-      <c r="C13" s="4">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="15">
-        <v>576</v>
-      </c>
-      <c r="C14" s="4">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="15">
+        <v>256</v>
+      </c>
+      <c r="C17" s="3">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="14">
+        <v>512</v>
+      </c>
+      <c r="C18" s="3">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="14">
+        <v>384</v>
+      </c>
+      <c r="C19" s="3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="14">
+        <v>488</v>
+      </c>
+      <c r="C20" s="3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="14">
+        <v>656</v>
+      </c>
+      <c r="C21" s="3">
         <v>608</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="15">
-        <v>960</v>
-      </c>
-      <c r="C15" s="4">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="3">
-        <v>256</v>
-      </c>
-      <c r="C16" s="4">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="15">
-        <v>512</v>
-      </c>
-      <c r="C17" s="4">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="15">
-        <v>384</v>
-      </c>
-      <c r="C18" s="4">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="15">
-        <v>488</v>
-      </c>
-      <c r="C19" s="4">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="15">
-        <v>656</v>
-      </c>
-      <c r="C20" s="4">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="5">
-        <v>1216</v>
-      </c>
-      <c r="C21" s="6">
-        <v>352</v>
+      <c r="B22" s="16">
+        <v>1180</v>
+      </c>
+      <c r="C22" s="5">
+        <v>380</v>
       </c>
     </row>
   </sheetData>

</xml_diff>